<commit_message>
Correction of calibration sheet
Formula had "+" instead of "-"
</commit_message>
<xml_diff>
--- a/v2.2/DStage_ETC_v2.2_calibration.xlsx
+++ b/v2.2/DStage_ETC_v2.2_calibration.xlsx
@@ -14,6 +14,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="51">
   <si>
+    <t>Calibration should be performed with throttle motor disconnected!</t>
+  </si>
+  <si>
     <t>Please fill in fielsd in</t>
   </si>
   <si>
@@ -23,10 +26,10 @@
     <t>info</t>
   </si>
   <si>
-    <t>Calibration procedure:</t>
-  </si>
-  <si>
-    <t>to be performed with throttle motor disconnected!</t>
+    <t>Calibration procedure to get you in the ball park:</t>
+  </si>
+  <si>
+    <t>Throttle</t>
   </si>
   <si>
     <r>
@@ -68,24 +71,24 @@
     </r>
   </si>
   <si>
-    <t>Throttle</t>
+    <t>Throttle sensor voltage when fully closed</t>
   </si>
   <si>
     <t>V</t>
   </si>
   <si>
-    <t>Throttle sensor voltage when fully closed</t>
-  </si>
-  <si>
     <t>input</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Step 2 - Connect the throttle input and with closed throttle use </t>
+    <t>Throttle sensor voltage when fully oppened</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Step 2 - with closed throttle use </t>
     </r>
     <r>
       <rPr>
@@ -119,7 +122,10 @@
     </r>
   </si>
   <si>
-    <t>Throttle sensor voltage when fully oppened</t>
+    <t>required gain for throttle input</t>
+  </si>
+  <si>
+    <t>result</t>
   </si>
   <si>
     <r>
@@ -146,12 +152,6 @@
     </r>
   </si>
   <si>
-    <t>required gain for throttle input</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
     <t>required offset for throttle input</t>
   </si>
   <si>
@@ -203,12 +203,27 @@
     <t>calculated</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Step 5 - Connect the gas pedal input and with it de-pressed use </t>
+    <t>target when closed</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Step 5 - with gas pedal de-pressed use PR3 to set the voltage at test point C to the below value</t>
+  </si>
+  <si>
+    <t>target when oppened</t>
+  </si>
+  <si>
+    <t>target range</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color theme="1"/>
+      </rPr>
+      <t xml:space="preserve">Step 6 - press the gas pedal and check voltage at test point </t>
     </r>
     <r>
       <rPr>
@@ -216,21 +231,6 @@
         <b/>
         <color theme="1"/>
       </rPr>
-      <t>PR3</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> to set the voltage at test point </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
       <t>C</t>
     </r>
     <r>
@@ -238,44 +238,8 @@
         <rFont val="Arial"/>
         <color theme="1"/>
       </rPr>
-      <t xml:space="preserve"> to the below value</t>
-    </r>
-  </si>
-  <si>
-    <t>target when closed</t>
-  </si>
-  <si>
-    <t>constant</t>
-  </si>
-  <si>
-    <t>target when oppened</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">Step 3 - press the gas pedal and check voltage at test point </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color theme="1"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
       <t>, it should be close to the below value</t>
     </r>
-  </si>
-  <si>
-    <t>target range</t>
   </si>
   <si>
     <t>series diode offset</t>
@@ -357,7 +321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -365,6 +329,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="12.0"/>
+      <color rgb="FFFF0000"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -376,10 +353,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11.0"/>
-      <color rgb="FFFF0000"/>
-      <name val="&quot;Google Sans&quot;"/>
+      <sz val="9.0"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Google Sans Mono&quot;"/>
     </font>
   </fonts>
   <fills count="13">
@@ -391,6 +367,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF1C232"/>
         <bgColor rgb="FFF1C232"/>
       </patternFill>
@@ -399,12 +381,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFF2CC"/>
         <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -462,57 +438,61 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="2" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="2" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="2" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="2" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="2" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="2" xfId="0" applyFill="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -738,359 +718,363 @@
     <col customWidth="1" min="3" max="3" width="4.5"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="5" t="s">
+    </row>
+    <row r="3">
+      <c r="G3" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="G3" s="3" t="s">
+    <row r="4">
+      <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6">
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.885</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="8">
         <f>B9</f>
-        <v>2.42</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1.4</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="8" t="s">
+        <v>2.571187181</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
-        <v>3.2</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="9">
+    </row>
+    <row r="7">
+      <c r="B7" s="10"/>
+      <c r="G7" s="11">
         <f>B12</f>
         <v>4</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="11" t="s">
+      <c r="B8" s="14">
+        <f>B14/B11</f>
+        <v>0.7761966365</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12">
-        <f>B14/B11</f>
-        <v>1.666666667</v>
-      </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="11" t="s">
+      <c r="G8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="9">
+    </row>
+    <row r="9">
+      <c r="A9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="14">
+        <f>(B12-B15+B8*B5)/(B8+1)</f>
+        <v>2.571187181</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="11">
         <f>B13</f>
         <v>1</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="12">
-        <f>(B12+B15+B8*B5)/(B8+1)</f>
-        <v>2.42</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="10"/>
+      <c r="G10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10">
-      <c r="G10" s="6">
+    <row r="11">
+      <c r="A11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="18">
+        <f>B6-B5</f>
+        <v>3.865</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="8">
         <f>B23</f>
-        <v>2.479238095</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="16">
-        <f>B6-B5</f>
-        <v>1.8</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="3" t="s">
+        <v>2.374095238</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="17" t="s">
+      <c r="B12" s="20">
+        <v>4.0</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="18">
-        <v>4.0</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="17" t="s">
+      <c r="G12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="9">
+    </row>
+    <row r="13">
+      <c r="A13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="11">
         <f>B26</f>
         <v>4</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="19">
+      <c r="B14" s="21">
         <f>B12-B13</f>
         <v>3</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="C14" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="20">
+        <v>0.12</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="11">
         <f>B27</f>
         <v>1.05</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="18">
-        <v>0.12</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>22</v>
+      <c r="H15" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="3">
         <v>1.2</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="3">
         <v>3.5</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22" s="14">
         <f>B28/B25</f>
         <v>1.282608696</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="11" t="s">
-        <v>14</v>
+      <c r="C22" s="15"/>
+      <c r="D22" s="13" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="12">
-        <f>(B26+B29+B22*B19)/(B22+1)</f>
-        <v>2.479238095</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="B23" s="14">
+        <f>(B26-B29+B22*B19)/(B22+1)</f>
+        <v>2.374095238</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="16">
+      <c r="B25" s="18">
         <f>B20-B19</f>
         <v>2.3</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="15" t="s">
+      <c r="C25" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="20">
         <v>4.0</v>
       </c>
-      <c r="C26" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>22</v>
+      <c r="C26" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="20">
         <v>1.05</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>22</v>
+      <c r="C27" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="19">
+      <c r="A28" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="21">
         <f>B26-B27</f>
         <v>2.95</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>22</v>
+      <c r="C28" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="20">
         <v>0.12</v>
       </c>
-      <c r="C29" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>22</v>
+      <c r="C29" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1109,171 +1093,171 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>1.28</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="4">
         <v>4.0</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
+      <c r="H2" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>2.5</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="4">
         <v>1.0</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="22">
         <f>G2-G3</f>
         <v>3</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>1.2</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>3.5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="4">
         <v>3.5</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
+      <c r="H6" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="4">
         <v>1.2</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
+      <c r="H7" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="22">
         <f t="shared" ref="B8:B9" si="1">B$2*(B$3-B5)+B$3</f>
         <v>4.164</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="22">
         <f>G6-G7</f>
         <v>2.3</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>7</v>
+      <c r="H8" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="22">
         <f t="shared" si="1"/>
         <v>1.22</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="23">
         <f>G4/G8</f>
         <v>1.304347826</v>
       </c>
     </row>
     <row r="11">
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="23">
         <f>G6*G10</f>
         <v>4.565217391</v>
       </c>
     </row>
     <row r="12">
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="23">
         <f>G7*G10</f>
         <v>1.565217391</v>
       </c>
     </row>
     <row r="13">
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="23">
         <f>G6*G10-G2</f>
         <v>0.5652173913</v>
       </c>
     </row>
     <row r="14">
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="23">
         <f>G7*G10-G3</f>
         <v>0.5652173913</v>
       </c>

</xml_diff>